<commit_message>
feat: schedule done, latest 24h
</commit_message>
<xml_diff>
--- a/reports.xlsx
+++ b/reports.xlsx
@@ -397,133 +397,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>nome</v>
-      </c>
-      <c r="B1" t="str">
-        <v>email</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Hora de entrada</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Hora de saída</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Sala</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>matheus</v>
-      </c>
-      <c r="B2" t="str">
-        <v>matheus@gmail.com</v>
-      </c>
-      <c r="C2" t="str">
-        <v>19:58</v>
-      </c>
-      <c r="D2" t="str">
-        <v>19:59</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Sala 1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>clerisson</v>
-      </c>
-      <c r="B3" t="str">
-        <v>clerisson@gmail.com</v>
-      </c>
-      <c r="C3" t="str">
-        <v>19:58</v>
-      </c>
-      <c r="D3" t="str">
-        <v>19:59</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Sala 1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Lucas</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Lucas@gmail.com</v>
-      </c>
-      <c r="C4" t="str">
-        <v>19:58</v>
-      </c>
-      <c r="D4" t="str">
-        <v>19:59</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Sala 1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>pikachu</v>
-      </c>
-      <c r="B5" t="str">
-        <v>pikachu@gmail.com</v>
-      </c>
-      <c r="C5" t="str">
-        <v>19:58</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Não informado</v>
-      </c>
-      <c r="E5" t="str">
-        <v>sala 3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>dragonball</v>
-      </c>
-      <c r="B6" t="str">
-        <v>dragonball@gmail.com</v>
-      </c>
-      <c r="C6" t="str">
-        <v>19:58</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Não informado</v>
-      </c>
-      <c r="E6" t="str">
-        <v>sala 3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>miau</v>
-      </c>
-      <c r="B7" t="str">
-        <v>miau@gmail.com</v>
-      </c>
-      <c r="C7" t="str">
-        <v>19:58</v>
-      </c>
-      <c r="D7" t="str">
-        <v>19:59</v>
-      </c>
-      <c r="E7" t="str">
-        <v>sala 3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>